<commit_message>
chỉnh lại ko dùng <p> cho xuống hàng
</commit_message>
<xml_diff>
--- a/imported_test_upload.xlsx
+++ b/imported_test_upload.xlsx
@@ -17,333 +17,283 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <r>
-      <t xml:space="preserve">description
+      <t>description</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <color/>
+      </rPr>
+      <t>in đậm</t>
+    </r>
+    <r>
+      <t xml:space="preserve">, test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <color/>
+      </rPr>
+      <t xml:space="preserve">in nghiệm, </t>
+    </r>
+    <r>
+      <t xml:space="preserve">test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t>underline</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <color/>
+      </rPr>
+      <t>in nghiệm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t>underline</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>text này là double underline</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test 1 chữ vừa </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <color/>
+      </rPr>
+      <t>in đâm vừa in nghiêm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test này là vừa </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <color/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t>in đậm vừa underline</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test này là vừa </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t>italic vừa underline</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test này cả </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t>3 thứ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>đây là chỗ có xuống dòng
+dòng 1
+dòng 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">đây là chỗ có xuống dòng in nghiêng, in đâm và underline
 </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t/>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">test này là </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <color/>
-      </rPr>
-      <t>in đậm</t>
-    </r>
-    <r>
-      <t xml:space="preserve">, test này là </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <color/>
-      </rPr>
-      <t xml:space="preserve">in nghiệm, </t>
-    </r>
-    <r>
-      <t xml:space="preserve">test này là </t>
-    </r>
-    <r>
-      <rPr>
-        <color/>
-        <u val="single"/>
-      </rPr>
-      <t>underline</t>
+    <r>
+      <rPr>
+        <b/>
+        <color/>
+      </rPr>
+      <t>dòng 1</t>
     </r>
     <r>
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">test này là </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <color/>
-      </rPr>
-      <t>in nghiệm</t>
+    <r>
+      <rPr>
+        <i/>
+        <color/>
+      </rPr>
+      <t>dòng 2</t>
     </r>
     <r>
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">test này là </t>
-    </r>
-    <r>
-      <rPr>
-        <color/>
-        <u val="single"/>
-      </rPr>
-      <t>underline</t>
+    <r>
+      <rPr>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t>dòng 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">đây là chỗ có xuống dòng in nghiêng, in đâm và underline
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <color/>
+      </rPr>
+      <t>dòng 1</t>
     </r>
     <r>
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">text này là double underline
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">test 1 chữ vừa </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <color/>
-      </rPr>
-      <t>in đâm vừa in nghiêm</t>
+    <r>
+      <rPr>
+        <i/>
+        <color/>
+      </rPr>
+      <t>dòng 2</t>
     </r>
     <r>
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">test này là vừa </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <color/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <color/>
-        <u val="single"/>
-      </rPr>
-      <t>in đậm vừa underline</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
+    <r>
+      <rPr>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t xml:space="preserve">dòng 3
 </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">test này là vừa </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <color/>
-        <u val="single"/>
-      </rPr>
-      <t>italic vừa underline</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">test này cả </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <color/>
-        <u val="single"/>
-      </rPr>
-      <t>3 thứ</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">đây là chỗ có xuống dòng
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t>dòng 4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <color/>
+      </rPr>
+      <t xml:space="preserve">in đậm.    </t>
+    </r>
+    <r>
+      <t xml:space="preserve">, test.     này là </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <color/>
+      </rPr>
+      <t xml:space="preserve">in      nghiệm.   , </t>
+    </r>
+    <r>
+      <t xml:space="preserve">test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t>underline</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">chỗ này là xuống 2 và </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t xml:space="preserve"> 3</t>
+    </r>
+    <r>
+      <t>dòng
 dòng 1
 dòng 2
+dòng 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <color/>
+      </rPr>
+      <t xml:space="preserve">ข้อมูลสินค้าเพิ่มเติม
 </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">đây là chỗ có xuống dòng in nghiêng, in đâm và underline
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <color/>
-      </rPr>
-      <t>dòng 1</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <color/>
-      </rPr>
-      <t>dòng 2</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <color/>
-        <u val="single"/>
-      </rPr>
-      <t>dòng 3</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">đây là chỗ có xuống dòng in nghiêng, in đâm và underline
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <color/>
-      </rPr>
-      <t>dòng 1</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <color/>
-      </rPr>
-      <t>dòng 2</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <color/>
-        <u val="single"/>
-      </rPr>
-      <t>dòng 3</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <color/>
-        <u val="single"/>
-      </rPr>
-      <t>dòng 4</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">test này là </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <color/>
-      </rPr>
-      <t xml:space="preserve">in đậm.    </t>
-    </r>
-    <r>
-      <t xml:space="preserve">, test.     này là </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <color/>
-      </rPr>
-      <t xml:space="preserve">in      nghiệm.   , </t>
-    </r>
-    <r>
-      <t xml:space="preserve">test này là </t>
-    </r>
-    <r>
-      <rPr>
-        <color/>
-        <u val="single"/>
-      </rPr>
-      <t>underline</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">chỗ này là xuống 2 và </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <color/>
-        <u val="single"/>
-      </rPr>
-      <t xml:space="preserve"> 3</t>
-    </r>
-    <r>
-      <t xml:space="preserve">dòng
-dòng 1
-dòng 2
-dòng 3
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <color/>
-      </rPr>
-      <t>ข้อมูลสินค้าเพิ่มเติม</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
     <r>
       <rPr>
         <b/>
@@ -353,7 +303,7 @@
       <t>-100%</t>
     </r>
     <r>
-      <t xml:space="preserve">Color
+      <t>Color 
 Volume Quantum Dot สีสวยสด 100%
 Quantum HDR เผยรายละเอียดที่ซ่อนอยุ่ในภาพ
 AirSlim ตัวเครื่องบาง  สวยงาม  ประหยัดพื้นที่
@@ -361,7 +311,7 @@
 คุณสมบัติเฉพาะ
 แบรนด์ : SAMSUNG
 ซีรีส์
-: Q65C
+ : Q65C
 ความสูง ( ซม .) : 64.41
 ความกว้าง ( ซม .) : 111.83
 ความลึก ( ซม .) : 2.57
@@ -385,20 +335,16 @@
 ข้อมูลการรับประกัน
 การรับประกัน ( ปี ) : 1
 ข้อมูลติดต่อศูนย์บริการ
-CALL CENTER 1282 บริษัท  ไทยซัมซุง  อิเลคโทรนิคส์  จำกัด  ศูนย์บริการเปิดให้บริการตั้งแต่วันจันทร์ถึงวันเสาร์ 9.00 17.00 น .
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ข้อมูลสินค้าเพิ่มเติม
-</t>
-    </r>
-    <r>
-      <t xml:space="preserve">-100% Color Volume Quantum Dot สีสวยสด 100%
+CALL CENTER 1282 บริษัท  ไทยซัมซุง  อิเลคโทรนิคส์  จำกัด  ศูนย์บริการเปิดให้บริการตั้งแต่วันจันทร์ถึงวันเสาร์ 9.00 17.00 น .</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ข้อมูลสินค้าเพิ่มเติม
+-100% Color Volume Quantum Dot สีสวยสด 100%
 Quantum HDR เผยรายละเอียดที่ซ่อนอยุ่ในภาพ
 AirSlim ตัวเครื่องบาง สวยงาม ประหยัดพื้นที่
-Smart Hub คัดสรรคอนเทนต์บันเทิงรวมไว้ในที่เดียว
+Smart Hub คัดสรรคอนเทนต์บันเทิงรวมไว้ในที่เดียว 
 คุณสมบัติเฉพาะ
 แบรนด์ : SAMSUNG
 ซีรีส์ : Q65C
@@ -407,7 +353,7 @@
 ความลึก (ซม.) : 2.57
 น้ำหนัก (กก.) : 10.7
 ขนาดหน้าจอ (นิ้ว) : 50"
-ความละเอียดหน้าจอ : 4K (3,840 x 2,160)
+ความละเอียดหน้าจอ : 4K (3,840 x 2,160) 
 ชนิดหน้าจอ : QLED
 DIGITAL TV BUILT IN (YES/NO) : YES
 SMART TV : TIZEN
@@ -425,8 +371,7 @@
 ข้อมูลการรับประกัน
 การรับประกัน (ปี) : 1
 ข้อมูลติดต่อศูนย์บริการ
-CALL CENTER 1282 บริษัท ไทยซัมซุง อิเลคโทรนิคส์ จำกัด ศูนย์บริการเปิดให้บริการตั้งแต่วันจันทร์ถึงวันเสาร์ 9.00 17.00 น.
-</t>
+CALL CENTER 1282 บริษัท ไทยซัมซุง อิเลคโทรนิคส์ จำกัด ศูนย์บริการเปิดให้บริการตั้งแต่วันจันทร์ถึงวันเสาร์ 9.00 17.00 น.</t>
     </r>
   </si>
 </sst>

</xml_diff>

<commit_message>
xử lý chuyển img sang link
</commit_message>
<xml_diff>
--- a/imported_test_upload.xlsx
+++ b/imported_test_upload.xlsx
@@ -279,8 +279,15 @@
       <t xml:space="preserve"> 3</t>
     </r>
     <r>
+      <rPr>
+        <color/>
+        <u val="single"/>
+      </rPr>
+      <t xml:space="preserve"> https://thisisimageurl.com </t>
+    </r>
+    <r>
       <t>dòng
-dòng 1
+dòng 1 
 dòng 2
 dòng 3</t>
     </r>
@@ -340,8 +347,8 @@
   </si>
   <si>
     <r>
-      <t>ข้อมูลสินค้าเพิ่มเติม
--100% Color Volume Quantum Dot สีสวยสด 100%
+      <t>111 ข้อมูลสินค้าเพิ่มเติม
+-100% https://thisisimageurl.com  Color Volume Quantum Dot สีสวยสด 100%
 Quantum HDR เผยรายละเอียดที่ซ่อนอยุ่ในภาพ
 AirSlim ตัวเครื่องบาง สวยงาม ประหยัดพื้นที่
 Smart Hub คัดสรรคอนเทนต์บันเทิงรวมไว้ในที่เดียว 

</xml_diff>